<commit_message>
Planilha cinemark segunda classificada Classifcador NB rudimentar (e falho) Primeira iteração pronta
</commit_message>
<xml_diff>
--- a/Cinemark segunda 16-03.xlsx
+++ b/Cinemark segunda 16-03.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive - Insper - Institudo de Ensino e Pesquisa\Desktop\Insper\2°Semestre DP\CDados\CD2020-Projeto1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/giovanniar_al_insper_edu_br/Documents/Desktop/Insper/2°Semestre DP/CDados/CD2020-Projeto1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{9C2E2897-1743-4CCE-83BD-DC03CBAA25AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{1BBCC188-4610-4FA3-ACF3-10C58EB19246}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="13_ncr:1_{9C2E2897-1743-4CCE-83BD-DC03CBAA25AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{051C234B-6B53-444D-9098-769C3DA63E9F}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2475" yWindow="1305" windowWidth="10245" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="314">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1084,6 +1084,9 @@
   </si>
   <si>
     <t>tenho uma cortesia pro cinemark que vence semana que vem, mas os cinemas fecharam por causa do corona vairus!</t>
+  </si>
+  <si>
+    <t>Opinião</t>
   </si>
 </sst>
 </file>
@@ -1150,12 +1153,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1494,20 +1498,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B251"/>
+  <dimension ref="A1:G251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1515,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1523,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1531,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1539,7 +1546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1547,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1555,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1563,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1571,7 +1578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1579,15 +1586,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1595,7 +1603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1603,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1611,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1619,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1684,7 +1692,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B24">
@@ -2031,901 +2039,1441 @@
       <c r="A67" t="s">
         <v>66</v>
       </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
+      </c>
+      <c r="B240">
+        <v>1</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
+      <c r="B241">
+        <v>1</v>
+      </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
+      <c r="B242">
+        <v>0</v>
+      </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
+      <c r="B243">
+        <v>0</v>
+      </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
+      <c r="B244">
+        <v>1</v>
+      </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
+      <c r="B245">
+        <v>1</v>
+      </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
+      <c r="B246">
+        <v>0</v>
+      </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
@@ -2969,7 +3517,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>